<commit_message>
minor changes for test purposes
</commit_message>
<xml_diff>
--- a/models/powerstation_coal/sysconfig_pscoal_600MW.xlsx
+++ b/models/powerstation_coal/sysconfig_pscoal_600MW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="16840" tabRatio="804" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="16840" tabRatio="804" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="component_list" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -3003,7 +3006,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3866,8 +3869,8 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4522,7 +4525,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>